<commit_message>
Customer / Login updates
</commit_message>
<xml_diff>
--- a/doc/LUV IN BOX - Carga Produtos - Exemplo.xlsx
+++ b/doc/LUV IN BOX - Carga Produtos - Exemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\git\Luvit\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B05C016-E7E4-493B-BDBC-5F8A96F1E586}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8E1923-5A85-4F98-98EC-86ADD5948412}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC05BCB3-DF0D-4D1A-8910-0BA967F61A4C}"/>
   </bookViews>
@@ -34,14 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">_x000D_
-</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -52,65 +45,104 @@
     <t>CategoryId</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
     <t>BarCode</t>
   </si>
   <si>
-    <t>Dimension.Width</t>
-  </si>
-  <si>
-    <t>Dimension.Height</t>
-  </si>
-  <si>
-    <t>Dimension.Length</t>
-  </si>
-  <si>
-    <t>Dimension.Weight</t>
-  </si>
-  <si>
-    <t>Image.Type</t>
-  </si>
-  <si>
-    <t>Image.Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sugador Womanizer Liberty</t>
-  </si>
-  <si>
-    <t>Sugador de Clitóris Liberty Pink</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1499.90</t>
-  </si>
-  <si>
-    <t>http://site.com.br/imagem.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sugador Free Women</t>
-  </si>
-  <si>
-    <t>Sugador de Clitóris Free Women Purpple</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1299.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /9j/4AAQSkZJRgABAQEAYABgAAD/4QC0RXhpZgAATU0AKgAAAAgABwExAAIAAAAiAAAAYgEyAAIAAAAUAAAAhAMBAAUAAAABAAAAmAMCAAIAAAAMAAAAoFEQAAEAAAABAQAAAFERAAQAAAABAAAOxFESAAQAAAABAAAOxAAAAABBZG9iZSBQaG90b3Nob3AgQ0MgMjAxOSAoV2luZG93cykAMjAyMTowMjowMSAwOTo0NDozOQAAAYagAACxjklDQyBQcm9maWxlAP/</t>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>CompleteDescription</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Care</t>
+  </si>
+  <si>
+    <t>PowerSupply</t>
+  </si>
+  <si>
+    <t>Maturity</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Sizes</t>
+  </si>
+  <si>
+    <t>PackageDimension</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>JonTComfPExt_3</t>
+  </si>
+  <si>
+    <t>Preservativo Jontex Comfort Plus Extra Lubrificado 3 Unidades</t>
+  </si>
+  <si>
+    <t>Descrição completa aceita formatação HTML</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>Descrição completa do uso do produto - aceita formatação HTML</t>
+  </si>
+  <si>
+    <t>Descrição completa do material aceita formatação HTML</t>
+  </si>
+  <si>
+    <t>Fabricante: Hypermarcas S/A.</t>
+  </si>
+  <si>
+    <t>Marca: Jontex</t>
+  </si>
+  <si>
+    <t>Descrição completa dos cuidados com o produto - aceita formatação HTML</t>
+  </si>
+  <si>
+    <t>Descrição completa sobre a fonte de alimentação / energia do produto aceita formatação HTML</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>Informaçãos sobre o vencimento do produto aceita formatação HTML</t>
+  </si>
+  <si>
+    <t>Código hexadecimal da cor do produto, ex: #FFFFFF (preto)</t>
+  </si>
+  <si>
+    <t>Largura, Altura, Comprimento, Peso, e Descrição, ex: {0,0,0,0, "Descrição"}</t>
+  </si>
+  <si>
+    <t>Passar entre colchetes, ex: [U, XL], valores posíveis: XS, S, M, L, XL, 2XL, 3XL, 4XL, U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,13 +150,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,12 +185,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,158 +504,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D76FE1-1B62-44F8-B821-4AEE2F3A46F8}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="87" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2">
-        <v>4251460611046</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2">
+        <v>7350075027604</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2">
-        <v>7258460611088</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>